<commit_message>
"added new file and changed excel"
</commit_message>
<xml_diff>
--- a/Production Tableau server Upgrade Checklist-10.5.3.xlsx
+++ b/Production Tableau server Upgrade Checklist-10.5.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viv6kor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Learnings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,9 +116,6 @@
     <t>Not tested</t>
   </si>
   <si>
-    <t>Amount of Data on the servers(Check for 1 main site AE)</t>
-  </si>
-  <si>
     <t>7.08 GB</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>PT7(Production)</t>
+  </si>
+  <si>
+    <t>Amount of Data on the server(Check for 1 main site AE)</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A2:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -720,13 +720,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>18</v>
@@ -756,13 +756,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>31</v>
-      </c>
       <c r="D13" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>18</v>
@@ -903,10 +903,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>18</v>
@@ -988,10 +988,10 @@
     <row r="26" spans="1:6" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>

</xml_diff>